<commit_message>
Set Google Credentials as Global Variable
</commit_message>
<xml_diff>
--- a/Data/2017_10_16/output_py.xlsx
+++ b/Data/2017_10_16/output_py.xlsx
@@ -3408,7 +3408,7 @@
     <t>Since the last update, &amp;quot;save image&amp;quot; is always popping up on image links, which is no longer &amp;quot;open in a new tab&amp;quot; when holding for longer, which was previously the case and eg Safari is still doing. Watched on iPhone 6 and 7.</t>
   </si>
   <si>
-    <t>I&amp;#39;m getting hacked by Hilton, she&amp;#39;s giving me murder tendencies why have you guys who I know have you fucked yourself with agents and your 13-year-old daughter is kidding with a man from the age of 60 and she walks at 1:00 At night alone, on the street home, where her mother is waiting for her to be able to use that child to be used. You are sick pointless and your toothless sister too. Marcel is acquainted with pool. Wiilemskade there you work to finish the job so far and that&amp;#39;s your room 15</t>
+    <t>I&amp;#39;m getting hacked by Hilton, she&amp;#39;s giving me murder tendencies why have you guys who I know have you fucked yourself with agents and your 13-year-old daughter is kidding with a man from the age of 60 and she walks at 1:00 At night alone, on the street home, where her mother is waiting for her to be able to use that child to be used. You are sick to nose and your toothless sister too. Marcel is acquainted with pool. Wiilemskade there you work to finish the job so far and that&amp;#39;s your room 15</t>
   </si>
   <si>
     <t>Hello dear Firefox Team, My bookmarks in the mobile Firefox version for iPhone (newest update) are suddenly all gone. Where are you going? I did not change anything, just opened the browser and they just were not there anymore. I do not have a Firefox account Can you please help me? Tibor.hettich@gmx.net Thank you, Tibor</t>
@@ -3483,7 +3483,7 @@
     <t>Lack of a handy gesture to expand, after all, the phone screen is getting bigger ~</t>
   </si>
   <si>
-    <t>It annoys me totally, if I click on a photo / graphic, every time a popup appears if I want to copy the memory or. No I do not want to! And if, then that happens rather seldom. Especially since you get away with a further click as cancel, otherwise no scroll or other goes! Please install a deactivation in the settings.</t>
+    <t>It annoys me totally, if I click on a photo / graphic, each time a popup appears if I want to copy the memory or. No I do not want to! And if, then that happens rather seldom. Especially since you get away with a further click as cancel, otherwise no scroll or other goes! Please install a deactivation in the settings.</t>
   </si>
   <si>
     <t>When browsing YouTube site for example, every moment when I&amp;#39;m passing the videos that are on the right side at all times it appears to &amp;quot;save image&amp;quot; and I do not want it I just want to pass the videos. That&amp;#39;s annoying. Over time you have to click outside to exit this save image and re-search for a video. Please remove that. I use a 4 Ger. With iOS 10. Thanks.</t>
@@ -4890,7 +4890,7 @@
     <t>[-0.30000001192092896, 0.10000000149011612, -0.8999999761581421, -0.800000011920929]</t>
   </si>
   <si>
-    <t>[-0.699999988079071, -0.800000011920929, 0.30000001192092896, 0.30000001192092896]</t>
+    <t>[-0.699999988079071, -0.4000000059604645, 0.30000001192092896, 0.30000001192092896]</t>
   </si>
   <si>
     <t>[-0.10000000149011612, -0.10000000149011612, -0.800000011920929, 0.20000000298023224, 0.4000000059604645]</t>
@@ -6030,7 +6030,7 @@
     <t>[0.30000001192092896, 0.10000000149011612, 0.8999999761581421, 0.800000011920929]</t>
   </si>
   <si>
-    <t>[0.699999988079071, 0.800000011920929, 0.30000001192092896, 0.30000001192092896]</t>
+    <t>[0.699999988079071, 0.4000000059604645, 0.30000001192092896, 0.30000001192092896]</t>
   </si>
   <si>
     <t>[0.10000000149011612, 0.10000000149011612, 0.800000011920929, 0.20000000298023224, 0.4000000059604645]</t>
@@ -7283,7 +7283,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -33058,10 +33058,10 @@
         <v>1074</v>
       </c>
       <c r="I610">
-        <v>-0.2000000029802322</v>
+        <v>-0.1000000014901161</v>
       </c>
       <c r="J610">
-        <v>0.5249999761581421</v>
+        <v>0.425000011920929</v>
       </c>
       <c r="K610" t="s">
         <v>1568</v>
@@ -33070,7 +33070,7 @@
         <v>1948</v>
       </c>
       <c r="M610" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="N610" t="s">
         <v>2020</v>

</xml_diff>

<commit_message>
Add Pause the programme to work with Google API
</commit_message>
<xml_diff>
--- a/Data/2017_10_16/output_py.xlsx
+++ b/Data/2017_10_16/output_py.xlsx
@@ -3081,7 +3081,7 @@
     <t>Bug report. Can not even open in the current version on the iPhone SE. Of course, the rating will be handled with troubleshooting. Firefox Clear, however, works flawlessly.</t>
   </si>
   <si>
-    <t>Needs improvement. * iOS 10.3.3 - iPhone 5s / iPad Air 1 * With the update, the app freezes constantly. One page just loaded, you will suddenly see everything in gray. Reload does not work. Only the complete close and reopen opens. Until it freezes again ... +++ 5.0 ++ If you log in on a page and or in the tab overview, the back function does not work anymore. Like having opened a new tab. Terrible ++ Unfortunately, the browser is a bit slow and Java sites like Amazon or eBay do not want to display the images properly or the images can not be wiped. In addition, the tabs are cumbersome. In the overview mode it jerky neat. The arrangement of the settings is also awkward. Something that is often used, such as clearing the history / cookies, continues to fall down. That&amp;#39;s higher! Completely wrong, I find the solution of the favorites, because when you start the browser you are in the history mode, unlike the Safari in Bookmark / Favorites mode. Even the favorite star in the bottom bar has gone. There is the tab switcher, because always maneuvering upwards is cumbersome, because the other actions are below ... Great I would also like to start the browser in private mode, unfortunately, you have to re-activate each time. In general, I&amp;#39;m looking forward to the Firefox, it was initially abandoned by Mozilla for iOS. Unfortunately, there is still a lot of room for improvement. Whether Apple&amp;#39;s third-party browser also allows to use AddOns like AdBlocks?</t>
+    <t>Needs improvement. * iOS 10.3.3 - iPhone 5s / iPad Air 1 * With the update, the app freezes constantly. One page just loaded, you will suddenly see everything in gray. Reload does not work. Only the complete close and reopen opens. Until it freezes again ... +++ 5.0 ++ If you log in on a page and or in the tab overview, the back function does not work anymore. Like having opened a new tab. Terrible ++ Unfortunately, the browser is a bit slow and Java sites like Amazon or eBay do not want to display the images properly or the images can not be wiped. In addition, the tabs are cumbersome. In the overview mode it jerky neat. The arrangement of the settings is also awkward. Something that is often used, such as clearing the history / cookies, continues to fall down. That&amp;#39;s higher! Completely wrong, I find the solution of the favorites, because when you start the browser you are in the history mode, unlike the Safari in Bookmark / Favorites mode. Even the favorite star in the bottom bar has gone. There is the tab switcher, because always maneuvering upwards is cumbersome, because the other actions are below ... Great I would also start the browser in private mode, unfortunately, you have to re-activate each time. In general, I&amp;#39;m looking forward to the Firefox, it was initially abandoned by Mozilla for iOS. Unfortunately, there is still a lot of room for improvement. Whether Apple&amp;#39;s third-party browser also allows to use AddOns like AdBlocks?</t>
   </si>
   <si>
     <t>Okay. Very nice</t>
@@ -3405,7 +3405,7 @@
     <t>I still can not get cookies active</t>
   </si>
   <si>
-    <t>Since the last update, &amp;quot;save image&amp;quot; is always popping up on image links, which is no longer &amp;quot;open in a new tab&amp;quot; when holding for longer, which was previously the case and eg Safari is still doing. Watched on iPhone 6 and 7.</t>
+    <t>Since the last update, &amp;quot;save image&amp;quot; is always popping up on image links, but what&amp;#39;s not happening is &amp;quot;opening in a new tab&amp;quot; for longer, which was previously the case and eg Safari is still doing. Watched on iPhone 6 and 7.</t>
   </si>
   <si>
     <t>I&amp;#39;m getting hacked by Hilton, she&amp;#39;s giving me murder tendencies why have you guys who I know have you fucked yourself with agents and your 13-year-old daughter is kidding with a man from the age of 60 and she walks at 1:00 At night alone, on the street home, where her mother is waiting for her to be able to use that child to be used. You are sick to nose and your toothless sister too. Marcel is acquainted with pool. Wiilemskade there you work to finish the job so far and that&amp;#39;s your room 15</t>
@@ -4308,7 +4308,7 @@
     <t>[0.800000011920929, 0.8999999761581421, 0.800000011920929]</t>
   </si>
   <si>
-    <t>[0.0, -0.8999999761581421, -0.10000000149011612, -0.8999999761581421, -0.20000000298023224, -0.6000000238418579, -0.699999988079071, 0.4000000059604645, -0.800000011920929, -0.5, 0.4000000059604645, -0.800000011920929, -0.20000000298023224, 0.0, -0.800000011920929, 0.30000001192092896, -0.5, 0.6000000238418579, -0.10000000149011612, 0.0, 0.20000000298023224]</t>
+    <t>[0.0, -0.8999999761581421, -0.10000000149011612, -0.8999999761581421, -0.20000000298023224, -0.6000000238418579, -0.699999988079071, 0.4000000059604645, -0.800000011920929, -0.5, 0.4000000059604645, -0.800000011920929, -0.20000000298023224, 0.0, -0.800000011920929, 0.30000001192092896, -0.5, 0.5, -0.10000000149011612, 0.0, 0.20000000298023224]</t>
   </si>
   <si>
     <t>[-0.800000011920929, -0.10000000149011612, -0.20000000298023224, -0.800000011920929, 0.800000011920929]</t>
@@ -5646,7 +5646,7 @@
     <t>[0.20000000298023224, 0.699999988079071, 0.0, 0.8999999761581421]</t>
   </si>
   <si>
-    <t>[0.0, 0.8999999761581421, 0.10000000149011612, 0.8999999761581421, 0.20000000298023224, 0.6000000238418579, 0.699999988079071, 0.4000000059604645, 0.800000011920929, 0.5, 0.4000000059604645, 0.800000011920929, 0.20000000298023224, 0.0, 0.800000011920929, 0.30000001192092896, 0.5, 0.6000000238418579, 0.10000000149011612, 0.0, 0.20000000298023224]</t>
+    <t>[0.0, 0.8999999761581421, 0.10000000149011612, 0.8999999761581421, 0.20000000298023224, 0.6000000238418579, 0.699999988079071, 0.4000000059604645, 0.800000011920929, 0.5, 0.4000000059604645, 0.800000011920929, 0.20000000298023224, 0.0, 0.800000011920929, 0.30000001192092896, 0.5, 0.5, 0.10000000149011612, 0.0, 0.20000000298023224]</t>
   </si>
   <si>
     <t>[0.800000011920929, 0.10000000149011612, 0.20000000298023224, 0.800000011920929, 0.800000011920929]</t>
@@ -19007,7 +19007,7 @@
         <v>-0.2000000029802322</v>
       </c>
       <c r="J267">
-        <v>0.4761904761904762</v>
+        <v>0.4714285532633464</v>
       </c>
       <c r="K267" t="s">
         <v>1374</v>

</xml_diff>

<commit_message>
Add stats of Components and Features
</commit_message>
<xml_diff>
--- a/Data/2017_10_16/output_py.xlsx
+++ b/Data/2017_10_16/output_py.xlsx
@@ -7,14 +7,16 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Component Count" sheetId="2" r:id="rId2"/>
+    <sheet name="Feature Count" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6917" uniqueCount="1912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6991" uniqueCount="1935">
   <si>
     <t>Store</t>
   </si>
@@ -5921,13 +5923,82 @@
   <si>
     <t>time, copi, option</t>
   </si>
+  <si>
+    <t># Reviews</t>
+  </si>
+  <si>
+    <t>Private Mode</t>
+  </si>
+  <si>
+    <t>Tracking Protection</t>
+  </si>
+  <si>
+    <t>Top Sites</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Reading List</t>
+  </si>
+  <si>
+    <t>Night Mode</t>
+  </si>
+  <si>
+    <t>Desktop View</t>
+  </si>
+  <si>
+    <t>QR code</t>
+  </si>
+  <si>
+    <t>Save Logins</t>
+  </si>
+  <si>
+    <t>Save image</t>
+  </si>
+  <si>
+    <t>Copy Image</t>
+  </si>
+  <si>
+    <t>Remove a page</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Copy link</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>View bookmarks</t>
+  </si>
+  <si>
+    <t>Set default mail</t>
+  </si>
+  <si>
+    <t>Request desktop site</t>
+  </si>
+  <si>
+    <t>Scan</t>
+  </si>
+  <si>
+    <t>Change/reset password</t>
+  </si>
+  <si>
+    <t>Look Up</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -32191,4 +32262,611 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B2">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B5">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B8">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B11">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B17">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B19">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B23">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B24">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B26">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>